<commit_message>
Added Spring server logic for uploading the file
</commit_message>
<xml_diff>
--- a/target/classes/time_report.xlsx
+++ b/target/classes/time_report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\Java\Projects\TravelDocumentProceeder\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E82F2707-F2F0-4023-9601-318939F8E8DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{296B4EA5-A0CB-4521-9438-D43595BD55D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6172,7 +6172,7 @@
   <dimension ref="A1:CL65536"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="C1" zoomScale="50" zoomScaleNormal="25" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <selection activeCell="BB3" sqref="BB3"/>
+      <selection activeCell="AR18" sqref="AR18:BL20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="28.5" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>